<commit_message>
b gniazda do sprawdzenia
</commit_message>
<xml_diff>
--- a/kable_gniazdka.xlsx
+++ b/kable_gniazdka.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="303">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="309">
   <si>
     <t xml:space="preserve">Budynek B </t>
   </si>
@@ -925,6 +925,24 @@
   </si>
   <si>
     <t>G_A1_56</t>
+  </si>
+  <si>
+    <t>odlegóść to od gniazda do przepustu na danym piętrze</t>
+  </si>
+  <si>
+    <t>G_B1_55</t>
+  </si>
+  <si>
+    <t>te polewo to mają -3 bo jak wyjdze ze stropu to można od razu ciągnać, nie trzeba do sufitu ich</t>
+  </si>
+  <si>
+    <t>17.75</t>
+  </si>
+  <si>
+    <t>18.41</t>
+  </si>
+  <si>
+    <t>G_B2_105</t>
   </si>
 </sst>
 </file>
@@ -961,13 +979,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1340,8 +1361,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N123"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="K52" sqref="K52:K75"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I109" sqref="I109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1432,16 +1453,23 @@
         <v>4</v>
       </c>
       <c r="B4" s="2">
-        <v>27.37</v>
+        <v>30.37</v>
       </c>
       <c r="C4" t="s">
         <v>52</v>
       </c>
-      <c r="D4" s="2"/>
+      <c r="D4" s="2">
+        <v>11.53</v>
+      </c>
       <c r="E4" t="s">
         <v>53</v>
       </c>
-      <c r="F4" s="2"/>
+      <c r="F4" s="2">
+        <v>11.34</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>305</v>
+      </c>
       <c r="H4" t="s">
         <v>213</v>
       </c>
@@ -1464,6 +1492,7 @@
         <v>109</v>
       </c>
       <c r="F5" s="2"/>
+      <c r="G5" s="3"/>
       <c r="H5" t="s">
         <v>215</v>
       </c>
@@ -1472,22 +1501,30 @@
         <v>247</v>
       </c>
       <c r="K5" s="2"/>
+      <c r="N5" t="s">
+        <v>303</v>
+      </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
       <c r="B6" s="2">
-        <v>26.03</v>
+        <v>29.03</v>
       </c>
       <c r="C6" t="s">
         <v>56</v>
       </c>
-      <c r="D6" s="2"/>
+      <c r="D6" s="2">
+        <v>9.58</v>
+      </c>
       <c r="E6" t="s">
         <v>110</v>
       </c>
-      <c r="F6" s="2"/>
+      <c r="F6" s="2">
+        <v>10.64</v>
+      </c>
+      <c r="G6" s="3"/>
       <c r="H6" t="s">
         <v>216</v>
       </c>
@@ -1510,6 +1547,7 @@
         <v>111</v>
       </c>
       <c r="F7" s="2"/>
+      <c r="G7" s="3"/>
       <c r="H7" t="s">
         <v>217</v>
       </c>
@@ -1523,15 +1561,22 @@
       <c r="A8" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="2"/>
+      <c r="B8" s="2">
+        <v>28.43</v>
+      </c>
       <c r="C8" t="s">
         <v>58</v>
       </c>
-      <c r="D8" s="2"/>
+      <c r="D8" s="2">
+        <v>20.87</v>
+      </c>
       <c r="E8" t="s">
         <v>112</v>
       </c>
-      <c r="F8" s="2"/>
+      <c r="F8" s="2">
+        <v>8.0399999999999991</v>
+      </c>
+      <c r="G8" s="3"/>
       <c r="H8" t="s">
         <v>218</v>
       </c>
@@ -1554,6 +1599,7 @@
         <v>113</v>
       </c>
       <c r="F9" s="2"/>
+      <c r="G9" s="3"/>
       <c r="H9" t="s">
         <v>219</v>
       </c>
@@ -1567,15 +1613,22 @@
       <c r="A10" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="2"/>
+      <c r="B10" s="2">
+        <v>29.23</v>
+      </c>
       <c r="C10" t="s">
         <v>60</v>
       </c>
-      <c r="D10" s="2"/>
+      <c r="D10" s="2">
+        <v>19.11</v>
+      </c>
       <c r="E10" t="s">
         <v>114</v>
       </c>
-      <c r="F10" s="2"/>
+      <c r="F10" s="2">
+        <v>7.39</v>
+      </c>
+      <c r="G10" s="3"/>
       <c r="H10" t="s">
         <v>220</v>
       </c>
@@ -1598,6 +1651,7 @@
         <v>115</v>
       </c>
       <c r="F11" s="2"/>
+      <c r="G11" s="3"/>
       <c r="H11" t="s">
         <v>221</v>
       </c>
@@ -1611,15 +1665,22 @@
       <c r="A12" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="2"/>
+      <c r="B12" s="2">
+        <v>24.5</v>
+      </c>
       <c r="C12" t="s">
         <v>62</v>
       </c>
-      <c r="D12" s="2"/>
+      <c r="D12" s="2">
+        <v>16.47</v>
+      </c>
       <c r="E12" t="s">
         <v>116</v>
       </c>
-      <c r="F12" s="2"/>
+      <c r="F12" s="2">
+        <v>6.04</v>
+      </c>
+      <c r="G12" s="3"/>
       <c r="H12" t="s">
         <v>222</v>
       </c>
@@ -1642,6 +1703,7 @@
         <v>117</v>
       </c>
       <c r="F13" s="2"/>
+      <c r="G13" s="3"/>
       <c r="H13" t="s">
         <v>223</v>
       </c>
@@ -1655,15 +1717,22 @@
       <c r="A14" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="2"/>
+      <c r="B14" s="2">
+        <v>23.93</v>
+      </c>
       <c r="C14" t="s">
         <v>64</v>
       </c>
-      <c r="D14" s="2"/>
+      <c r="D14" s="2">
+        <v>12.86</v>
+      </c>
       <c r="E14" t="s">
         <v>118</v>
       </c>
-      <c r="F14" s="2"/>
+      <c r="F14" s="2">
+        <v>5.51</v>
+      </c>
+      <c r="G14" s="3"/>
       <c r="H14" t="s">
         <v>224</v>
       </c>
@@ -1686,6 +1755,7 @@
         <v>119</v>
       </c>
       <c r="F15" s="2"/>
+      <c r="G15" s="3"/>
       <c r="H15" t="s">
         <v>225</v>
       </c>
@@ -1699,15 +1769,22 @@
       <c r="A16" t="s">
         <v>16</v>
       </c>
-      <c r="B16" s="2"/>
+      <c r="B16" s="2">
+        <v>25.68</v>
+      </c>
       <c r="C16" t="s">
         <v>66</v>
       </c>
-      <c r="D16" s="2"/>
+      <c r="D16" s="2">
+        <v>17.100000000000001</v>
+      </c>
       <c r="E16" t="s">
         <v>120</v>
       </c>
-      <c r="F16" s="2"/>
+      <c r="F16" s="2">
+        <v>6.79</v>
+      </c>
+      <c r="G16" s="3"/>
       <c r="H16" t="s">
         <v>226</v>
       </c>
@@ -1730,6 +1807,7 @@
         <v>121</v>
       </c>
       <c r="F17" s="2"/>
+      <c r="G17" s="3"/>
       <c r="H17" t="s">
         <v>227</v>
       </c>
@@ -1743,15 +1821,22 @@
       <c r="A18" t="s">
         <v>18</v>
       </c>
-      <c r="B18" s="2"/>
+      <c r="B18" s="2">
+        <v>20.16</v>
+      </c>
       <c r="C18" t="s">
         <v>68</v>
       </c>
-      <c r="D18" s="2"/>
+      <c r="D18" s="2">
+        <v>24.05</v>
+      </c>
       <c r="E18" t="s">
         <v>122</v>
       </c>
-      <c r="F18" s="2"/>
+      <c r="F18" s="2">
+        <v>7.34</v>
+      </c>
+      <c r="G18" s="3"/>
       <c r="H18" t="s">
         <v>228</v>
       </c>
@@ -1774,6 +1859,7 @@
         <v>123</v>
       </c>
       <c r="F19" s="2"/>
+      <c r="G19" s="3"/>
       <c r="H19" t="s">
         <v>229</v>
       </c>
@@ -1787,15 +1873,21 @@
       <c r="A20" t="s">
         <v>20</v>
       </c>
-      <c r="B20" s="2"/>
+      <c r="B20" s="2">
+        <v>16.16</v>
+      </c>
       <c r="C20" t="s">
         <v>70</v>
       </c>
-      <c r="D20" s="2"/>
+      <c r="D20" s="2">
+        <v>20.95</v>
+      </c>
       <c r="E20" t="s">
         <v>124</v>
       </c>
-      <c r="F20" s="2"/>
+      <c r="F20" s="2">
+        <v>14.39</v>
+      </c>
       <c r="H20" t="s">
         <v>230</v>
       </c>
@@ -1831,15 +1923,21 @@
       <c r="A22" t="s">
         <v>22</v>
       </c>
-      <c r="B22" s="2"/>
+      <c r="B22" s="2">
+        <v>15.45</v>
+      </c>
       <c r="C22" t="s">
         <v>72</v>
       </c>
-      <c r="D22" s="2"/>
+      <c r="D22" s="2">
+        <v>24.52</v>
+      </c>
       <c r="E22" t="s">
         <v>126</v>
       </c>
-      <c r="F22" s="2"/>
+      <c r="F22" s="2">
+        <v>15.12</v>
+      </c>
       <c r="H22" t="s">
         <v>232</v>
       </c>
@@ -1875,15 +1973,21 @@
       <c r="A24" t="s">
         <v>24</v>
       </c>
-      <c r="B24" s="2"/>
+      <c r="B24" s="2">
+        <v>13.48</v>
+      </c>
       <c r="C24" t="s">
         <v>74</v>
       </c>
-      <c r="D24" s="2"/>
+      <c r="D24" s="2">
+        <v>25.02</v>
+      </c>
       <c r="E24" t="s">
         <v>128</v>
       </c>
-      <c r="F24" s="2"/>
+      <c r="F24" s="2">
+        <v>15.79</v>
+      </c>
       <c r="H24" t="s">
         <v>234</v>
       </c>
@@ -1919,15 +2023,21 @@
       <c r="A26" t="s">
         <v>26</v>
       </c>
-      <c r="B26" s="2"/>
+      <c r="B26" s="2">
+        <v>12.66</v>
+      </c>
       <c r="C26" t="s">
         <v>76</v>
       </c>
-      <c r="D26" s="2"/>
+      <c r="D26" s="2">
+        <v>27.12</v>
+      </c>
       <c r="E26" t="s">
         <v>130</v>
       </c>
-      <c r="F26" s="2"/>
+      <c r="F26" s="2">
+        <v>18.45</v>
+      </c>
       <c r="H26" t="s">
         <v>236</v>
       </c>
@@ -1963,15 +2073,21 @@
       <c r="A28" t="s">
         <v>28</v>
       </c>
-      <c r="B28" s="2"/>
+      <c r="B28" s="2">
+        <v>7.71</v>
+      </c>
       <c r="C28" t="s">
         <v>78</v>
       </c>
-      <c r="D28" s="2"/>
+      <c r="D28" s="2">
+        <v>27.42</v>
+      </c>
       <c r="E28" t="s">
         <v>132</v>
       </c>
-      <c r="F28" s="2"/>
+      <c r="F28" s="2">
+        <v>21.09</v>
+      </c>
       <c r="H28" t="s">
         <v>238</v>
       </c>
@@ -2007,15 +2123,21 @@
       <c r="A30" t="s">
         <v>30</v>
       </c>
-      <c r="B30" s="2"/>
+      <c r="B30" s="2">
+        <v>13.05</v>
+      </c>
       <c r="C30" t="s">
         <v>80</v>
       </c>
-      <c r="D30" s="2"/>
+      <c r="D30" s="2">
+        <v>29.62</v>
+      </c>
       <c r="E30" t="s">
         <v>134</v>
       </c>
-      <c r="F30" s="2"/>
+      <c r="F30" s="2">
+        <v>21.74</v>
+      </c>
       <c r="H30" t="s">
         <v>240</v>
       </c>
@@ -2051,15 +2173,21 @@
       <c r="A32" t="s">
         <v>32</v>
       </c>
-      <c r="B32" s="2"/>
+      <c r="B32" s="2">
+        <v>15.93</v>
+      </c>
       <c r="C32" t="s">
         <v>82</v>
       </c>
-      <c r="D32" s="2"/>
+      <c r="D32" s="2">
+        <v>30.12</v>
+      </c>
       <c r="E32" t="s">
         <v>136</v>
       </c>
-      <c r="F32" s="2"/>
+      <c r="F32" s="2">
+        <v>22.44</v>
+      </c>
       <c r="H32" t="s">
         <v>242</v>
       </c>
@@ -2095,15 +2223,21 @@
       <c r="A34" t="s">
         <v>34</v>
       </c>
-      <c r="B34" s="2"/>
+      <c r="B34" s="2">
+        <v>18.23</v>
+      </c>
       <c r="C34" t="s">
         <v>84</v>
       </c>
-      <c r="D34" s="2"/>
+      <c r="D34" s="2">
+        <v>33.630000000000003</v>
+      </c>
       <c r="E34" t="s">
         <v>138</v>
       </c>
-      <c r="F34" s="2"/>
+      <c r="F34" s="2">
+        <v>23.19</v>
+      </c>
       <c r="H34" t="s">
         <v>244</v>
       </c>
@@ -2139,15 +2273,21 @@
       <c r="A36" t="s">
         <v>36</v>
       </c>
-      <c r="B36" s="2"/>
+      <c r="B36" s="2">
+        <v>20.63</v>
+      </c>
       <c r="C36" t="s">
         <v>86</v>
       </c>
-      <c r="D36" s="2"/>
+      <c r="D36" s="2">
+        <v>35.83</v>
+      </c>
       <c r="E36" t="s">
         <v>140</v>
       </c>
-      <c r="F36" s="2"/>
+      <c r="F36" s="2">
+        <v>37.26</v>
+      </c>
       <c r="H36" t="s">
         <v>246</v>
       </c>
@@ -2180,15 +2320,21 @@
       <c r="A38" t="s">
         <v>38</v>
       </c>
-      <c r="B38" s="2"/>
+      <c r="B38" s="2">
+        <v>22.18</v>
+      </c>
       <c r="C38" t="s">
         <v>88</v>
       </c>
-      <c r="D38" s="2"/>
+      <c r="D38" s="2">
+        <v>39.520000000000003</v>
+      </c>
       <c r="E38" t="s">
         <v>142</v>
       </c>
-      <c r="F38" s="2"/>
+      <c r="F38" s="2">
+        <v>36.75</v>
+      </c>
       <c r="I38" s="2"/>
       <c r="J38" t="s">
         <v>280</v>
@@ -2218,15 +2364,21 @@
       <c r="A40" t="s">
         <v>40</v>
       </c>
-      <c r="B40" s="2"/>
+      <c r="B40" s="2">
+        <v>23.83</v>
+      </c>
       <c r="C40" t="s">
         <v>90</v>
       </c>
-      <c r="D40" s="2"/>
+      <c r="D40" s="2">
+        <v>38.020000000000003</v>
+      </c>
       <c r="E40" t="s">
         <v>144</v>
       </c>
-      <c r="F40" s="2"/>
+      <c r="F40" s="2">
+        <v>36.29</v>
+      </c>
       <c r="I40" s="2"/>
       <c r="J40" t="s">
         <v>282</v>
@@ -2256,15 +2408,21 @@
       <c r="A42" t="s">
         <v>42</v>
       </c>
-      <c r="B42" s="2"/>
+      <c r="B42" s="2">
+        <v>21.33</v>
+      </c>
       <c r="C42" t="s">
         <v>92</v>
       </c>
-      <c r="D42" s="2"/>
+      <c r="D42" s="2">
+        <v>33.99</v>
+      </c>
       <c r="E42" t="s">
         <v>146</v>
       </c>
-      <c r="F42" s="2"/>
+      <c r="F42" s="2">
+        <v>34.74</v>
+      </c>
       <c r="I42" s="2"/>
       <c r="J42" t="s">
         <v>284</v>
@@ -2294,15 +2452,21 @@
       <c r="A44" t="s">
         <v>44</v>
       </c>
-      <c r="B44" s="2"/>
+      <c r="B44" s="2">
+        <v>23.93</v>
+      </c>
       <c r="C44" t="s">
         <v>94</v>
       </c>
-      <c r="D44" s="2"/>
+      <c r="D44" s="2">
+        <v>33.46</v>
+      </c>
       <c r="E44" t="s">
         <v>148</v>
       </c>
-      <c r="F44" s="2"/>
+      <c r="F44" s="2">
+        <v>34.270000000000003</v>
+      </c>
       <c r="I44" s="2"/>
       <c r="J44" t="s">
         <v>286</v>
@@ -2332,15 +2496,21 @@
       <c r="A46" t="s">
         <v>46</v>
       </c>
-      <c r="B46" s="2"/>
+      <c r="B46" s="2">
+        <v>25.63</v>
+      </c>
       <c r="C46" t="s">
         <v>96</v>
       </c>
-      <c r="D46" s="2"/>
+      <c r="D46" s="2">
+        <v>31.56</v>
+      </c>
       <c r="E46" t="s">
         <v>150</v>
       </c>
-      <c r="F46" s="2"/>
+      <c r="F46" s="2">
+        <v>33.770000000000003</v>
+      </c>
       <c r="I46" s="2"/>
       <c r="J46" t="s">
         <v>288</v>
@@ -2370,15 +2540,21 @@
       <c r="A48" t="s">
         <v>48</v>
       </c>
-      <c r="B48" s="2"/>
+      <c r="B48" s="2">
+        <v>28.13</v>
+      </c>
       <c r="C48" t="s">
         <v>98</v>
       </c>
-      <c r="D48" s="2"/>
+      <c r="D48" s="2">
+        <v>31.07</v>
+      </c>
       <c r="E48" t="s">
         <v>152</v>
       </c>
-      <c r="F48" s="2"/>
+      <c r="F48" s="2">
+        <v>32.11</v>
+      </c>
       <c r="I48" s="2"/>
       <c r="J48" t="s">
         <v>290</v>
@@ -2409,11 +2585,15 @@
       <c r="C50" t="s">
         <v>100</v>
       </c>
-      <c r="D50" s="2"/>
+      <c r="D50" s="2">
+        <v>29.07</v>
+      </c>
       <c r="E50" t="s">
         <v>154</v>
       </c>
-      <c r="F50" s="2"/>
+      <c r="F50" s="2">
+        <v>31.67</v>
+      </c>
       <c r="I50" s="2"/>
       <c r="J50" t="s">
         <v>292</v>
@@ -2441,11 +2621,15 @@
       <c r="C52" t="s">
         <v>102</v>
       </c>
-      <c r="D52" s="2"/>
+      <c r="D52" s="2">
+        <v>28.54</v>
+      </c>
       <c r="E52" t="s">
         <v>156</v>
       </c>
-      <c r="F52" s="2"/>
+      <c r="F52" s="2">
+        <v>41.23</v>
+      </c>
       <c r="J52" t="s">
         <v>294</v>
       </c>
@@ -2471,11 +2655,15 @@
       <c r="C54" t="s">
         <v>104</v>
       </c>
-      <c r="D54" s="2"/>
+      <c r="D54" s="2">
+        <v>28.42</v>
+      </c>
       <c r="E54" t="s">
         <v>158</v>
       </c>
-      <c r="F54" s="2"/>
+      <c r="F54" s="2">
+        <v>40.729999999999997</v>
+      </c>
       <c r="J54" t="s">
         <v>296</v>
       </c>
@@ -2500,11 +2688,15 @@
       <c r="C56" t="s">
         <v>106</v>
       </c>
-      <c r="D56" s="2"/>
+      <c r="D56" s="2">
+        <v>23.99</v>
+      </c>
       <c r="E56" t="s">
         <v>160</v>
       </c>
-      <c r="F56" s="2"/>
+      <c r="F56" s="2">
+        <v>40.24</v>
+      </c>
       <c r="J56" t="s">
         <v>298</v>
       </c>
@@ -2528,17 +2720,24 @@
       <c r="C58" t="s">
         <v>108</v>
       </c>
-      <c r="D58" s="2"/>
+      <c r="D58" s="2">
+        <v>19.420000000000002</v>
+      </c>
       <c r="E58" t="s">
         <v>162</v>
       </c>
-      <c r="F58" s="2"/>
+      <c r="F58" s="2">
+        <v>38.68</v>
+      </c>
       <c r="J58" t="s">
         <v>300</v>
       </c>
       <c r="K58" s="2"/>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C59" t="s">
+        <v>304</v>
+      </c>
       <c r="D59" s="2"/>
       <c r="E59" t="s">
         <v>163</v>
@@ -2554,7 +2753,9 @@
       <c r="E60" t="s">
         <v>164</v>
       </c>
-      <c r="F60" s="2"/>
+      <c r="F60" s="2">
+        <v>38.18</v>
+      </c>
       <c r="J60" t="s">
         <v>302</v>
       </c>
@@ -2573,7 +2774,9 @@
       <c r="E62" t="s">
         <v>166</v>
       </c>
-      <c r="F62" s="2"/>
+      <c r="F62" s="2">
+        <v>37.78</v>
+      </c>
       <c r="K62" s="2"/>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.25">
@@ -2589,7 +2792,9 @@
       <c r="E64" t="s">
         <v>168</v>
       </c>
-      <c r="F64" s="2"/>
+      <c r="F64" s="2">
+        <v>36.200000000000003</v>
+      </c>
       <c r="K64" s="2"/>
     </row>
     <row r="65" spans="4:11" x14ac:dyDescent="0.25">
@@ -2605,7 +2810,9 @@
       <c r="E66" t="s">
         <v>170</v>
       </c>
-      <c r="F66" s="2"/>
+      <c r="F66" s="2">
+        <v>35.78</v>
+      </c>
       <c r="K66" s="2"/>
     </row>
     <row r="67" spans="4:11" x14ac:dyDescent="0.25">
@@ -2621,7 +2828,9 @@
       <c r="E68" t="s">
         <v>172</v>
       </c>
-      <c r="F68" s="2"/>
+      <c r="F68" s="2">
+        <v>23.4</v>
+      </c>
       <c r="K68" s="2"/>
     </row>
     <row r="69" spans="4:11" x14ac:dyDescent="0.25">
@@ -2637,7 +2846,9 @@
       <c r="E70" t="s">
         <v>174</v>
       </c>
-      <c r="F70" s="2"/>
+      <c r="F70" s="2">
+        <v>22.54</v>
+      </c>
       <c r="K70" s="2"/>
     </row>
     <row r="71" spans="4:11" x14ac:dyDescent="0.25">
@@ -2653,7 +2864,9 @@
       <c r="E72" t="s">
         <v>176</v>
       </c>
-      <c r="F72" s="2"/>
+      <c r="F72" s="2">
+        <v>26.29</v>
+      </c>
       <c r="K72" s="2"/>
     </row>
     <row r="73" spans="4:11" x14ac:dyDescent="0.25">
@@ -2669,7 +2882,9 @@
       <c r="E74" t="s">
         <v>178</v>
       </c>
-      <c r="F74" s="2"/>
+      <c r="F74" s="2">
+        <v>27.08</v>
+      </c>
       <c r="K74" s="2"/>
     </row>
     <row r="75" spans="4:11" x14ac:dyDescent="0.25">
@@ -2684,7 +2899,9 @@
       <c r="E76" t="s">
         <v>180</v>
       </c>
-      <c r="F76" s="2"/>
+      <c r="F76" s="2">
+        <v>17.07</v>
+      </c>
     </row>
     <row r="77" spans="4:11" x14ac:dyDescent="0.25">
       <c r="E77" t="s">
@@ -2696,7 +2913,9 @@
       <c r="E78" t="s">
         <v>182</v>
       </c>
-      <c r="F78" s="2"/>
+      <c r="F78" s="2">
+        <v>16.11</v>
+      </c>
     </row>
     <row r="79" spans="4:11" x14ac:dyDescent="0.25">
       <c r="E79" t="s">
@@ -2708,7 +2927,9 @@
       <c r="E80" t="s">
         <v>184</v>
       </c>
-      <c r="F80" s="2"/>
+      <c r="F80" s="2">
+        <v>15.16</v>
+      </c>
     </row>
     <row r="81" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E81" t="s">
@@ -2720,7 +2941,9 @@
       <c r="E82" t="s">
         <v>186</v>
       </c>
-      <c r="F82" s="2"/>
+      <c r="F82" s="2">
+        <v>14.21</v>
+      </c>
     </row>
     <row r="83" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E83" t="s">
@@ -2732,7 +2955,9 @@
       <c r="E84" t="s">
         <v>188</v>
       </c>
-      <c r="F84" s="2"/>
+      <c r="F84" s="2">
+        <v>7.49</v>
+      </c>
     </row>
     <row r="85" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E85" t="s">
@@ -2744,7 +2969,9 @@
       <c r="E86" t="s">
         <v>190</v>
       </c>
-      <c r="F86" s="2"/>
+      <c r="F86" s="2">
+        <v>8.09</v>
+      </c>
     </row>
     <row r="87" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E87" t="s">
@@ -2756,7 +2983,9 @@
       <c r="E88" t="s">
         <v>192</v>
       </c>
-      <c r="F88" s="2"/>
+      <c r="F88" s="2">
+        <v>8.69</v>
+      </c>
     </row>
     <row r="89" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E89" t="s">
@@ -2768,7 +2997,9 @@
       <c r="E90" t="s">
         <v>194</v>
       </c>
-      <c r="F90" s="2"/>
+      <c r="F90" s="2">
+        <v>9.3000000000000007</v>
+      </c>
     </row>
     <row r="91" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E91" t="s">
@@ -2780,7 +3011,9 @@
       <c r="E92" t="s">
         <v>196</v>
       </c>
-      <c r="F92" s="2"/>
+      <c r="F92" s="2" t="s">
+        <v>306</v>
+      </c>
     </row>
     <row r="93" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E93" t="s">
@@ -2792,7 +3025,9 @@
       <c r="E94" t="s">
         <v>198</v>
       </c>
-      <c r="F94" s="2"/>
+      <c r="F94" s="2" t="s">
+        <v>307</v>
+      </c>
     </row>
     <row r="95" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E95" t="s">
@@ -2804,7 +3039,9 @@
       <c r="E96" t="s">
         <v>200</v>
       </c>
-      <c r="F96" s="2"/>
+      <c r="F96" s="2">
+        <v>19</v>
+      </c>
     </row>
     <row r="97" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E97" t="s">
@@ -2816,7 +3053,9 @@
       <c r="E98" t="s">
         <v>202</v>
       </c>
-      <c r="F98" s="2"/>
+      <c r="F98" s="2">
+        <v>19.68</v>
+      </c>
     </row>
     <row r="99" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E99" t="s">
@@ -2828,7 +3067,9 @@
       <c r="E100" t="s">
         <v>204</v>
       </c>
-      <c r="F100" s="2"/>
+      <c r="F100" s="2">
+        <v>22.54</v>
+      </c>
     </row>
     <row r="101" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E101" t="s">
@@ -2840,7 +3081,9 @@
       <c r="E102" t="s">
         <v>206</v>
       </c>
-      <c r="F102" s="2"/>
+      <c r="F102" s="2">
+        <v>23.44</v>
+      </c>
     </row>
     <row r="103" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E103" t="s">
@@ -2852,7 +3095,9 @@
       <c r="E104" t="s">
         <v>208</v>
       </c>
-      <c r="F104" s="2"/>
+      <c r="F104" s="2">
+        <v>24.34</v>
+      </c>
     </row>
     <row r="105" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E105" t="s">
@@ -2864,7 +3109,9 @@
       <c r="E106" t="s">
         <v>210</v>
       </c>
-      <c r="F106" s="2"/>
+      <c r="F106" s="2">
+        <v>25.25</v>
+      </c>
     </row>
     <row r="107" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E107" t="s">
@@ -2876,9 +3123,14 @@
       <c r="E108" t="s">
         <v>212</v>
       </c>
-      <c r="F108" s="2"/>
+      <c r="F108" s="2">
+        <v>16.489999999999998</v>
+      </c>
     </row>
     <row r="109" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E109" t="s">
+        <v>308</v>
+      </c>
       <c r="F109" s="2"/>
     </row>
     <row r="110" spans="5:6" x14ac:dyDescent="0.25">
@@ -2924,7 +3176,8 @@
       <c r="F123" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="189">
+  <mergeCells count="190">
+    <mergeCell ref="G4:G19"/>
     <mergeCell ref="K64:K65"/>
     <mergeCell ref="K66:K67"/>
     <mergeCell ref="K68:K69"/>

</xml_diff>